<commit_message>
CIERRE 15 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE   HERRADURA  FEBRERO   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE   HERRADURA  FEBRERO   2022.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="135">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -532,6 +532,24 @@
   </si>
   <si>
     <t>BALANCE      ABASTO 4 CARNES    H E R R A D U R A    FEBRERO          2 0 2 2</t>
+  </si>
+  <si>
+    <t>JAMON-VARIOS</t>
+  </si>
+  <si>
+    <t>NOMINA # 6</t>
+  </si>
+  <si>
+    <t>TOCINO-BOLA-RETAZO-QUESOS-JAMON</t>
+  </si>
+  <si>
+    <t>LONGANIZA-ARABE-JAMON</t>
+  </si>
+  <si>
+    <t>NOMINA # 7</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -904,7 +922,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -971,6 +989,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="59">
     <border>
@@ -1701,7 +1725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2086,6 +2110,87 @@
     <xf numFmtId="164" fontId="2" fillId="6" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="6" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="11" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="44" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="3" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2119,87 +2224,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="44" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="3" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3370,23 +3396,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="206"/>
-      <c r="C1" s="208" t="s">
+      <c r="B1" s="233"/>
+      <c r="C1" s="235" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="209"/>
-      <c r="I1" s="209"/>
-      <c r="J1" s="209"/>
-      <c r="K1" s="209"/>
-      <c r="L1" s="209"/>
-      <c r="M1" s="209"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="207"/>
+      <c r="B2" s="234"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -3396,21 +3422,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="210" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="211"/>
+      <c r="B3" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="238"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="212" t="s">
+      <c r="H3" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="212"/>
+      <c r="I3" s="239"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="217" t="s">
+      <c r="R3" s="206" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3425,14 +3451,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="213" t="s">
+      <c r="E4" s="240" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="H4" s="215" t="s">
+      <c r="F4" s="241"/>
+      <c r="H4" s="242" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="216"/>
+      <c r="I4" s="243"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -3442,11 +3468,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="213" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="225"/>
-      <c r="R4" s="218"/>
+      <c r="Q4" s="214"/>
+      <c r="R4" s="207"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -4927,11 +4953,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="226">
+      <c r="M40" s="215">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="228">
+      <c r="N40" s="217">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -4957,8 +4983,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="227"/>
-      <c r="N41" s="229"/>
+      <c r="M41" s="216"/>
+      <c r="N41" s="218"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -5173,29 +5199,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="230" t="s">
+      <c r="H53" s="219" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="231"/>
+      <c r="I53" s="220"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="232">
+      <c r="K53" s="221">
         <f>I51+L51</f>
         <v>44516.57</v>
       </c>
-      <c r="L53" s="233"/>
-      <c r="M53" s="234">
+      <c r="L53" s="222"/>
+      <c r="M53" s="223">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="235"/>
+      <c r="N53" s="224"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="236" t="s">
+      <c r="D54" s="225" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="236"/>
+      <c r="E54" s="225"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1567048.43</v>
@@ -5206,22 +5232,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="237" t="s">
+      <c r="D55" s="226" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="237"/>
+      <c r="E55" s="226"/>
       <c r="F55" s="115">
         <v>-1540248.71</v>
       </c>
-      <c r="I55" s="238" t="s">
+      <c r="I55" s="227" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="239"/>
-      <c r="K55" s="240">
+      <c r="J55" s="228"/>
+      <c r="K55" s="229">
         <f>F57+F58+F59</f>
         <v>181424.23999999996</v>
       </c>
-      <c r="L55" s="241"/>
+      <c r="L55" s="230"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -5252,11 +5278,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="242">
+      <c r="K57" s="231">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="243"/>
+      <c r="L57" s="232"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -5273,22 +5299,22 @@
       <c r="C59" s="133">
         <v>44591</v>
       </c>
-      <c r="D59" s="219" t="s">
+      <c r="D59" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="220"/>
+      <c r="E59" s="209"/>
       <c r="F59" s="134">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="221" t="s">
+      <c r="I59" s="210" t="s">
         <v>125</v>
       </c>
-      <c r="J59" s="222"/>
-      <c r="K59" s="223">
+      <c r="J59" s="211"/>
+      <c r="K59" s="212">
         <f>K55+K57</f>
         <v>-39635.46000000005</v>
       </c>
-      <c r="L59" s="223"/>
+      <c r="L59" s="212"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -5432,6 +5458,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
@@ -5447,12 +5479,6 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7252,10 +7278,10 @@
   <sheetPr>
     <tabColor rgb="FFFF66CC"/>
   </sheetPr>
-  <dimension ref="A1:S81"/>
+  <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7277,24 +7303,24 @@
     <col min="18" max="18" width="14.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="206"/>
-      <c r="C1" s="208" t="s">
+    <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="233"/>
+      <c r="C1" s="235" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="209"/>
-      <c r="E1" s="209"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="209"/>
-      <c r="H1" s="209"/>
-      <c r="I1" s="209"/>
-      <c r="J1" s="209"/>
-      <c r="K1" s="209"/>
-      <c r="L1" s="209"/>
-      <c r="M1" s="209"/>
-    </row>
-    <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="207"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+    </row>
+    <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="234"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -7303,26 +7329,26 @@
       <c r="M2" s="6"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="210" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="211"/>
+    <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="238"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="212" t="s">
+      <c r="H3" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="212"/>
+      <c r="I3" s="239"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="217" t="s">
+      <c r="R3" s="206" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -7333,14 +7359,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="213" t="s">
+      <c r="E4" s="240" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="H4" s="215" t="s">
+      <c r="F4" s="241"/>
+      <c r="H4" s="242" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="216"/>
+      <c r="I4" s="243"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -7350,13 +7376,13 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="224" t="s">
+      <c r="P4" s="213" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="225"/>
-      <c r="R4" s="218"/>
-    </row>
-    <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q4" s="214"/>
+      <c r="R4" s="207"/>
+    </row>
+    <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>8</v>
       </c>
@@ -7404,7 +7430,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="25">
         <v>44593</v>
@@ -7417,35 +7443,36 @@
         <v>44593</v>
       </c>
       <c r="F6" s="29">
-        <v>0</v>
+        <v>42378</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="37">
         <v>44593</v>
       </c>
       <c r="I6" s="31">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J6" s="38"/>
       <c r="K6" s="39"/>
       <c r="L6" s="40"/>
       <c r="M6" s="32">
-        <v>0</v>
+        <f>9692+32500</f>
+        <v>42192</v>
       </c>
       <c r="N6" s="33">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="34">
         <f t="shared" ref="P6:P39" si="0">N6+M6+L6+I6+C6</f>
-        <v>0</v>
+        <v>42378</v>
       </c>
       <c r="Q6" s="13">
         <v>0</v>
       </c>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="25">
         <v>44594</v>
@@ -7458,20 +7485,23 @@
         <v>44594</v>
       </c>
       <c r="F7" s="29">
-        <v>0</v>
+        <v>47132</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="37">
         <v>44594</v>
       </c>
       <c r="I7" s="31">
-        <v>0</v>
-      </c>
-      <c r="J7" s="38"/>
+        <v>186</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>8</v>
+      </c>
       <c r="K7" s="42"/>
       <c r="L7" s="40"/>
       <c r="M7" s="32">
-        <v>0</v>
+        <f>34300+12646</f>
+        <v>46946</v>
       </c>
       <c r="N7" s="33">
         <v>0</v>
@@ -7479,14 +7509,14 @@
       <c r="O7" s="2"/>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47132</v>
       </c>
       <c r="Q7" s="9">
         <v>0</v>
       </c>
       <c r="R7" s="9"/>
     </row>
-    <row r="8" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="25">
         <v>44595</v>
@@ -7499,7 +7529,7 @@
         <v>44595</v>
       </c>
       <c r="F8" s="29">
-        <v>0</v>
+        <v>65082</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="37">
@@ -7512,7 +7542,8 @@
       <c r="K8" s="45"/>
       <c r="L8" s="40"/>
       <c r="M8" s="32">
-        <v>0</v>
+        <f>30682+34400</f>
+        <v>65082</v>
       </c>
       <c r="N8" s="33">
         <v>0</v>
@@ -7520,7 +7551,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>65082</v>
       </c>
       <c r="Q8" s="9">
         <f t="shared" ref="Q8:Q39" si="1">P8-F8</f>
@@ -7528,41 +7559,44 @@
       </c>
       <c r="R8" s="9"/>
     </row>
-    <row r="9" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="25">
         <v>44596</v>
       </c>
       <c r="C9" s="26">
-        <v>0</v>
-      </c>
-      <c r="D9" s="41"/>
+        <v>12482</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>129</v>
+      </c>
       <c r="E9" s="28">
         <v>44596</v>
       </c>
       <c r="F9" s="29">
-        <v>0</v>
+        <v>71591</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="37">
         <v>44596</v>
       </c>
       <c r="I9" s="31">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J9" s="38"/>
       <c r="K9" s="46"/>
       <c r="L9" s="40"/>
       <c r="M9" s="32">
-        <v>0</v>
+        <f>28100+24178</f>
+        <v>52278</v>
       </c>
       <c r="N9" s="33">
-        <v>0</v>
+        <v>6800</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="34">
         <f>N9+M9+L9+I9+C9</f>
-        <v>0</v>
+        <v>71591</v>
       </c>
       <c r="Q9" s="9">
         <f>P9-F9</f>
@@ -7570,7 +7604,7 @@
       </c>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="25">
         <v>44597</v>
@@ -7583,49 +7617,61 @@
         <v>44597</v>
       </c>
       <c r="F10" s="29">
-        <v>0</v>
+        <v>73744</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="37">
         <v>44597</v>
       </c>
       <c r="I10" s="31">
-        <v>0</v>
-      </c>
-      <c r="J10" s="38"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="48"/>
+        <v>77</v>
+      </c>
+      <c r="J10" s="38">
+        <v>44597</v>
+      </c>
+      <c r="K10" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10" s="48">
+        <v>7950</v>
+      </c>
       <c r="M10" s="32">
-        <v>0</v>
+        <f>26061+38200</f>
+        <v>64261</v>
       </c>
       <c r="N10" s="33">
-        <v>0</v>
+        <v>1456</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73744</v>
       </c>
       <c r="Q10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R10" s="9"/>
-    </row>
-    <row r="11" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="25">
         <v>44598</v>
       </c>
       <c r="C11" s="26">
-        <v>0</v>
-      </c>
-      <c r="D11" s="36"/>
+        <v>5501</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>131</v>
+      </c>
       <c r="E11" s="28">
         <v>44598</v>
       </c>
       <c r="F11" s="29">
-        <v>0</v>
+        <v>79345</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="37">
@@ -7638,23 +7684,26 @@
       <c r="K11" s="49"/>
       <c r="L11" s="40"/>
       <c r="M11" s="32">
-        <v>0</v>
+        <f>64900+1644</f>
+        <v>66544</v>
       </c>
       <c r="N11" s="33">
-        <v>0</v>
+        <v>7300</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="34">
         <f>N11+M11+L11+I11+C11</f>
-        <v>0</v>
+        <v>79345</v>
       </c>
       <c r="Q11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R11" s="8"/>
-    </row>
-    <row r="12" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R11" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="25">
         <v>44599</v>
@@ -7667,36 +7716,37 @@
         <v>44599</v>
       </c>
       <c r="F12" s="29">
-        <v>0</v>
+        <v>67731</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="37">
         <v>44599</v>
       </c>
       <c r="I12" s="31">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J12" s="38"/>
       <c r="K12" s="50"/>
       <c r="L12" s="40"/>
       <c r="M12" s="32">
-        <v>0</v>
+        <f>13164</f>
+        <v>13164</v>
       </c>
       <c r="N12" s="33">
         <v>0</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="245"/>
       <c r="P12" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13231</v>
+      </c>
+      <c r="Q12" s="244">
+        <f t="shared" si="1"/>
+        <v>-54500</v>
       </c>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="25">
         <v>44600</v>
@@ -7709,28 +7759,29 @@
         <v>44600</v>
       </c>
       <c r="F13" s="29">
-        <v>0</v>
+        <v>51979</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="37">
         <v>44600</v>
       </c>
       <c r="I13" s="31">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
       <c r="M13" s="32">
-        <v>0</v>
+        <f>21751+29500</f>
+        <v>51251</v>
       </c>
       <c r="N13" s="33">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>51979</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" si="1"/>
@@ -7738,49 +7789,52 @@
       </c>
       <c r="R13" s="185"/>
     </row>
-    <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="25">
         <v>44601</v>
       </c>
       <c r="C14" s="26">
-        <v>0</v>
-      </c>
-      <c r="D14" s="51"/>
+        <v>6305</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>132</v>
+      </c>
       <c r="E14" s="28">
         <v>44601</v>
       </c>
       <c r="F14" s="29">
-        <v>0</v>
+        <v>41680</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="37">
         <v>44601</v>
       </c>
       <c r="I14" s="31">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J14" s="38"/>
       <c r="K14" s="45"/>
       <c r="L14" s="40"/>
       <c r="M14" s="32">
-        <v>0</v>
+        <f>16400+18750</f>
+        <v>35150</v>
       </c>
       <c r="N14" s="33">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41683</v>
       </c>
       <c r="Q14" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R14" s="185"/>
     </row>
-    <row r="15" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="25">
         <v>44602</v>
@@ -7793,7 +7847,7 @@
         <v>44602</v>
       </c>
       <c r="F15" s="29">
-        <v>0</v>
+        <v>63053</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="37">
@@ -7806,14 +7860,15 @@
       <c r="K15" s="45"/>
       <c r="L15" s="40"/>
       <c r="M15" s="32">
-        <v>0</v>
+        <f>38100+24952+1</f>
+        <v>63053</v>
       </c>
       <c r="N15" s="33">
         <v>0</v>
       </c>
       <c r="P15" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>63053</v>
       </c>
       <c r="Q15" s="13">
         <f t="shared" si="1"/>
@@ -7821,46 +7876,51 @@
       </c>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="25">
         <v>44603</v>
       </c>
       <c r="C16" s="26">
-        <v>0</v>
-      </c>
-      <c r="D16" s="36"/>
+        <v>18244</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="E16" s="28">
         <v>44603</v>
       </c>
       <c r="F16" s="29">
-        <v>0</v>
+        <v>76646</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="37">
         <v>44603</v>
       </c>
       <c r="I16" s="31">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="45"/>
       <c r="L16" s="9"/>
       <c r="M16" s="32">
-        <v>0</v>
+        <f>32669+25700</f>
+        <v>58369</v>
       </c>
       <c r="N16" s="33">
         <v>0</v>
       </c>
       <c r="P16" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76646</v>
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R16" s="8"/>
+      <c r="R16" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
@@ -7875,31 +7935,38 @@
         <v>44604</v>
       </c>
       <c r="F17" s="29">
-        <v>0</v>
+        <v>64635</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="37">
         <v>44604</v>
       </c>
       <c r="I17" s="31">
-        <v>0</v>
-      </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="48"/>
+        <v>22</v>
+      </c>
+      <c r="J17" s="38">
+        <v>44604</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="L17" s="48">
+        <v>10085.709999999999</v>
+      </c>
       <c r="M17" s="32">
-        <v>0</v>
+        <f>18624+32500</f>
+        <v>51124</v>
       </c>
       <c r="N17" s="33">
-        <v>0</v>
+        <v>3403</v>
       </c>
       <c r="P17" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>64634.71</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.29000000000087311</v>
       </c>
       <c r="R17" s="8"/>
     </row>
@@ -7916,27 +7983,28 @@
         <v>44605</v>
       </c>
       <c r="F18" s="29">
-        <v>0</v>
+        <v>108725</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="37">
         <v>44605</v>
       </c>
       <c r="I18" s="31">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J18" s="38"/>
       <c r="K18" s="53"/>
       <c r="L18" s="40"/>
       <c r="M18" s="32">
-        <v>0</v>
+        <f>18700+37100+47000+4577</f>
+        <v>107377</v>
       </c>
       <c r="N18" s="33">
-        <v>0</v>
+        <v>1305</v>
       </c>
       <c r="P18" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>108725</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="1"/>
@@ -7957,31 +8025,33 @@
         <v>44606</v>
       </c>
       <c r="F19" s="29">
-        <v>0</v>
+        <v>47223</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="37">
         <v>44606</v>
       </c>
       <c r="I19" s="31">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="J19" s="38"/>
       <c r="K19" s="54"/>
       <c r="L19" s="55"/>
       <c r="M19" s="32">
-        <v>0</v>
+        <f>30000</f>
+        <v>30000</v>
       </c>
       <c r="N19" s="33">
-        <v>0</v>
-      </c>
+        <v>860</v>
+      </c>
+      <c r="O19" s="245"/>
       <c r="P19" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30912</v>
+      </c>
+      <c r="Q19" s="244">
+        <f t="shared" si="1"/>
+        <v>-16311</v>
       </c>
       <c r="R19" s="8"/>
     </row>
@@ -8049,7 +8119,9 @@
         <v>0</v>
       </c>
       <c r="J21" s="38"/>
-      <c r="K21" s="57"/>
+      <c r="K21" s="57" t="s">
+        <v>134</v>
+      </c>
       <c r="L21" s="48"/>
       <c r="M21" s="32">
         <v>0</v>
@@ -8737,21 +8809,21 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="226">
+      <c r="M40" s="215">
         <f>SUM(M5:M39)</f>
-        <v>30643</v>
-      </c>
-      <c r="N40" s="228">
+        <v>777434</v>
+      </c>
+      <c r="N40" s="217">
         <f>SUM(N5:N39)</f>
-        <v>0</v>
+        <v>22148</v>
       </c>
       <c r="P40" s="34">
         <f>SUM(P5:P39)</f>
-        <v>35429</v>
+        <v>865564.71</v>
       </c>
       <c r="Q40" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>0</v>
+        <v>-70808.290000000008</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8767,8 +8839,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="227"/>
-      <c r="N41" s="229"/>
+      <c r="M41" s="216"/>
+      <c r="N41" s="218"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -8941,7 +9013,7 @@
       </c>
       <c r="C51" s="106">
         <f>SUM(C5:C50)</f>
-        <v>4540</v>
+        <v>47072</v>
       </c>
       <c r="D51" s="107"/>
       <c r="E51" s="108" t="s">
@@ -8949,7 +9021,7 @@
       </c>
       <c r="F51" s="109">
         <f>SUM(F5:F50)</f>
-        <v>35119</v>
+        <v>936063</v>
       </c>
       <c r="G51" s="107"/>
       <c r="H51" s="110" t="s">
@@ -8957,7 +9029,7 @@
       </c>
       <c r="I51" s="111">
         <f>SUM(I5:I50)</f>
-        <v>246</v>
+        <v>875</v>
       </c>
       <c r="J51" s="112"/>
       <c r="K51" s="113" t="s">
@@ -8965,7 +9037,7 @@
       </c>
       <c r="L51" s="114">
         <f>SUM(L5:L50)</f>
-        <v>0</v>
+        <v>18035.71</v>
       </c>
       <c r="M51" s="115"/>
       <c r="N51" s="115"/>
@@ -8983,32 +9055,32 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="230" t="s">
+      <c r="H53" s="219" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="231"/>
+      <c r="I53" s="220"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="232">
+      <c r="K53" s="221">
         <f>I51+L51</f>
-        <v>246</v>
-      </c>
-      <c r="L53" s="233"/>
-      <c r="M53" s="234">
+        <v>18910.71</v>
+      </c>
+      <c r="L53" s="222"/>
+      <c r="M53" s="223">
         <f>N40+M40</f>
-        <v>30643</v>
-      </c>
-      <c r="N53" s="235"/>
+        <v>799582</v>
+      </c>
+      <c r="N53" s="224"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="236" t="s">
+      <c r="D54" s="225" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="236"/>
+      <c r="E54" s="225"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
-        <v>30333</v>
+        <v>870080.29</v>
       </c>
       <c r="I54" s="121"/>
       <c r="J54" s="122"/>
@@ -9016,22 +9088,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="237" t="s">
+      <c r="D55" s="226" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="237"/>
+      <c r="E55" s="226"/>
       <c r="F55" s="115">
         <v>-1540248.71</v>
       </c>
-      <c r="I55" s="238" t="s">
+      <c r="I55" s="227" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="239"/>
-      <c r="K55" s="240">
+      <c r="J55" s="228"/>
+      <c r="K55" s="229">
         <f>F57+F58+F59</f>
-        <v>-1355291.19</v>
-      </c>
-      <c r="L55" s="241"/>
+        <v>-515543.89999999991</v>
+      </c>
+      <c r="L55" s="230"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -9055,18 +9127,18 @@
       </c>
       <c r="F57" s="115">
         <f>SUM(F54:F56)</f>
-        <v>-1509915.71</v>
+        <v>-670168.41999999993</v>
       </c>
       <c r="H57" s="24"/>
       <c r="I57" s="129" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="242">
+      <c r="K57" s="231">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="243"/>
+      <c r="L57" s="232"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -9083,22 +9155,22 @@
       <c r="C59" s="133">
         <v>44591</v>
       </c>
-      <c r="D59" s="219" t="s">
+      <c r="D59" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="220"/>
+      <c r="E59" s="209"/>
       <c r="F59" s="134">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="221" t="s">
+      <c r="I59" s="210" t="s">
         <v>125</v>
       </c>
-      <c r="J59" s="222"/>
-      <c r="K59" s="223">
+      <c r="J59" s="211"/>
+      <c r="K59" s="212">
         <f>K55+K57</f>
-        <v>-1509605.71</v>
-      </c>
-      <c r="L59" s="223"/>
+        <v>-669858.41999999993</v>
+      </c>
+      <c r="L59" s="212"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -9242,20 +9314,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="M53:N53"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
@@ -9263,6 +9321,20 @@
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="K59:L59"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="M53:N53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 7 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE   HERRADURA  FEBRERO   2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #02  FEBRERO 2022/BALANCE   HERRADURA  FEBRERO   2022.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="138">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -2113,6 +2113,39 @@
     <xf numFmtId="164" fontId="2" fillId="6" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="6" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="11" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="44" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2192,39 +2225,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3397,23 +3397,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="233"/>
-      <c r="C1" s="235" t="s">
+      <c r="B1" s="206"/>
+      <c r="C1" s="208" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="236"/>
-      <c r="K1" s="236"/>
-      <c r="L1" s="236"/>
-      <c r="M1" s="236"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="209"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="234"/>
+      <c r="B2" s="207"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -3423,21 +3423,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="237" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="238"/>
+      <c r="B3" s="210" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="211"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="239" t="s">
+      <c r="H3" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="239"/>
+      <c r="I3" s="212"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="206" t="s">
+      <c r="R3" s="217" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3452,14 +3452,14 @@
       <c r="D4" s="18">
         <v>44563</v>
       </c>
-      <c r="E4" s="240" t="s">
+      <c r="E4" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="241"/>
-      <c r="H4" s="242" t="s">
+      <c r="F4" s="214"/>
+      <c r="H4" s="215" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="243"/>
+      <c r="I4" s="216"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -3469,11 +3469,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="213" t="s">
+      <c r="P4" s="224" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="207"/>
+      <c r="Q4" s="225"/>
+      <c r="R4" s="218"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -4954,11 +4954,11 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="215">
+      <c r="M40" s="226">
         <f>SUM(M5:M39)</f>
         <v>1527030</v>
       </c>
-      <c r="N40" s="217">
+      <c r="N40" s="228">
         <f>SUM(N5:N39)</f>
         <v>50013</v>
       </c>
@@ -4984,8 +4984,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="216"/>
-      <c r="N41" s="218"/>
+      <c r="M41" s="227"/>
+      <c r="N41" s="229"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -5200,29 +5200,29 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="219" t="s">
+      <c r="H53" s="230" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="220"/>
+      <c r="I53" s="231"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="221">
+      <c r="K53" s="232">
         <f>I51+L51</f>
         <v>44516.57</v>
       </c>
-      <c r="L53" s="222"/>
-      <c r="M53" s="223">
+      <c r="L53" s="233"/>
+      <c r="M53" s="234">
         <f>N40+M40</f>
         <v>1577043</v>
       </c>
-      <c r="N53" s="224"/>
+      <c r="N53" s="235"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="225" t="s">
+      <c r="D54" s="236" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="225"/>
+      <c r="E54" s="236"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
         <v>1567048.43</v>
@@ -5233,22 +5233,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="226" t="s">
+      <c r="D55" s="237" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="226"/>
+      <c r="E55" s="237"/>
       <c r="F55" s="115">
         <v>-1540248.71</v>
       </c>
-      <c r="I55" s="227" t="s">
+      <c r="I55" s="238" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="228"/>
-      <c r="K55" s="229">
+      <c r="J55" s="239"/>
+      <c r="K55" s="240">
         <f>F57+F58+F59</f>
         <v>181424.23999999996</v>
       </c>
-      <c r="L55" s="230"/>
+      <c r="L55" s="241"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -5279,11 +5279,11 @@
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="231">
+      <c r="K57" s="242">
         <f>-C4</f>
         <v>-221059.7</v>
       </c>
-      <c r="L57" s="232"/>
+      <c r="L57" s="243"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -5300,22 +5300,22 @@
       <c r="C59" s="133">
         <v>44591</v>
       </c>
-      <c r="D59" s="208" t="s">
+      <c r="D59" s="219" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="209"/>
+      <c r="E59" s="220"/>
       <c r="F59" s="134">
         <v>154314.51999999999</v>
       </c>
-      <c r="I59" s="210" t="s">
+      <c r="I59" s="221" t="s">
         <v>125</v>
       </c>
-      <c r="J59" s="211"/>
-      <c r="K59" s="212">
+      <c r="J59" s="222"/>
+      <c r="K59" s="223">
         <f>K55+K57</f>
         <v>-39635.46000000005</v>
       </c>
-      <c r="L59" s="212"/>
+      <c r="L59" s="223"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -5459,12 +5459,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="I59:J59"/>
@@ -5480,6 +5474,12 @@
     <mergeCell ref="I55:J55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7281,8 +7281,8 @@
   </sheetPr>
   <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7305,23 +7305,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="233"/>
-      <c r="C1" s="235" t="s">
+      <c r="B1" s="206"/>
+      <c r="C1" s="208" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="236"/>
-      <c r="E1" s="236"/>
-      <c r="F1" s="236"/>
-      <c r="G1" s="236"/>
-      <c r="H1" s="236"/>
-      <c r="I1" s="236"/>
-      <c r="J1" s="236"/>
-      <c r="K1" s="236"/>
-      <c r="L1" s="236"/>
-      <c r="M1" s="236"/>
+      <c r="D1" s="209"/>
+      <c r="E1" s="209"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="209"/>
+      <c r="H1" s="209"/>
+      <c r="I1" s="209"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
+      <c r="M1" s="209"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="234"/>
+      <c r="B2" s="207"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -7331,21 +7331,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="237" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="238"/>
+      <c r="B3" s="210" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="211"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="239" t="s">
+      <c r="H3" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="239"/>
+      <c r="I3" s="212"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="R3" s="206" t="s">
+      <c r="R3" s="217" t="s">
         <v>38</v>
       </c>
     </row>
@@ -7360,14 +7360,14 @@
       <c r="D4" s="18">
         <v>44591</v>
       </c>
-      <c r="E4" s="240" t="s">
+      <c r="E4" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="241"/>
-      <c r="H4" s="242" t="s">
+      <c r="F4" s="214"/>
+      <c r="H4" s="215" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="243"/>
+      <c r="I4" s="216"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="21"/>
@@ -7377,11 +7377,11 @@
       <c r="N4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="213" t="s">
+      <c r="P4" s="224" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="207"/>
+      <c r="Q4" s="225"/>
+      <c r="R4" s="218"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
@@ -8594,14 +8594,16 @@
         <v>44619</v>
       </c>
       <c r="C32" s="26">
-        <v>0</v>
-      </c>
-      <c r="D32" s="78"/>
+        <v>18265</v>
+      </c>
+      <c r="D32" s="78" t="s">
+        <v>49</v>
+      </c>
       <c r="E32" s="28">
         <v>44619</v>
       </c>
       <c r="F32" s="29">
-        <v>0</v>
+        <v>112057</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="37">
@@ -8614,18 +8616,19 @@
       <c r="K32" s="74"/>
       <c r="L32" s="75"/>
       <c r="M32" s="32">
-        <v>0</v>
+        <f>45000+35000+9120</f>
+        <v>89120</v>
       </c>
       <c r="N32" s="33">
-        <v>0</v>
+        <v>4667</v>
       </c>
       <c r="P32" s="34">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>112052</v>
+      </c>
+      <c r="Q32" s="43">
+        <f t="shared" si="1"/>
+        <v>-5</v>
       </c>
       <c r="R32" s="8"/>
     </row>
@@ -8842,21 +8845,21 @@
       <c r="J40" s="73"/>
       <c r="K40" s="89"/>
       <c r="L40" s="75"/>
-      <c r="M40" s="215">
+      <c r="M40" s="226">
         <f>SUM(M5:M39)</f>
-        <v>1546988</v>
-      </c>
-      <c r="N40" s="217">
+        <v>1636108</v>
+      </c>
+      <c r="N40" s="228">
         <f>SUM(N5:N39)</f>
-        <v>51008</v>
+        <v>55675</v>
       </c>
       <c r="P40" s="34">
         <f>SUM(P5:P39)</f>
-        <v>1709187.21</v>
+        <v>1821239.21</v>
       </c>
       <c r="Q40" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>14.209999999999127</v>
+        <v>9.2099999999991269</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8872,8 +8875,8 @@
       <c r="J41" s="73"/>
       <c r="K41" s="76"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="216"/>
-      <c r="N41" s="218"/>
+      <c r="M41" s="227"/>
+      <c r="N41" s="229"/>
       <c r="P41" s="34"/>
       <c r="Q41" s="9"/>
     </row>
@@ -9046,7 +9049,7 @@
       </c>
       <c r="C51" s="106">
         <f>SUM(C5:C50)</f>
-        <v>70578</v>
+        <v>88843</v>
       </c>
       <c r="D51" s="107"/>
       <c r="E51" s="108" t="s">
@@ -9054,7 +9057,7 @@
       </c>
       <c r="F51" s="109">
         <f>SUM(F5:F50)</f>
-        <v>1708863</v>
+        <v>1820920</v>
       </c>
       <c r="G51" s="107"/>
       <c r="H51" s="110" t="s">
@@ -9088,32 +9091,32 @@
       <c r="A53" s="117"/>
       <c r="B53" s="118"/>
       <c r="C53" s="1"/>
-      <c r="H53" s="219" t="s">
+      <c r="H53" s="230" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="220"/>
+      <c r="I53" s="231"/>
       <c r="J53" s="119"/>
-      <c r="K53" s="221">
+      <c r="K53" s="232">
         <f>I51+L51</f>
         <v>40613.21</v>
       </c>
-      <c r="L53" s="222"/>
-      <c r="M53" s="223">
+      <c r="L53" s="233"/>
+      <c r="M53" s="234">
         <f>N40+M40</f>
-        <v>1597996</v>
-      </c>
-      <c r="N53" s="224"/>
+        <v>1691783</v>
+      </c>
+      <c r="N53" s="235"/>
       <c r="P53" s="34"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="225" t="s">
+      <c r="D54" s="236" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="225"/>
+      <c r="E54" s="236"/>
       <c r="F54" s="120">
         <f>F51-K53-C51</f>
-        <v>1597671.79</v>
+        <v>1691463.79</v>
       </c>
       <c r="I54" s="121"/>
       <c r="J54" s="122"/>
@@ -9121,22 +9124,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="226" t="s">
+      <c r="D55" s="237" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="226"/>
+      <c r="E55" s="237"/>
       <c r="F55" s="115">
-        <v>-1540248.71</v>
-      </c>
-      <c r="I55" s="227" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" s="238" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="228"/>
-      <c r="K55" s="229">
+      <c r="J55" s="239"/>
+      <c r="K55" s="240">
         <f>F57+F58+F59</f>
-        <v>212047.60000000006</v>
-      </c>
-      <c r="L55" s="230"/>
+        <v>1875805.98</v>
+      </c>
+      <c r="L55" s="241"/>
       <c r="P55" s="34"/>
       <c r="Q55" s="9"/>
     </row>
@@ -9160,18 +9163,18 @@
       </c>
       <c r="F57" s="115">
         <f>SUM(F54:F56)</f>
-        <v>57423.080000000075</v>
+        <v>1691463.79</v>
       </c>
       <c r="H57" s="24"/>
       <c r="I57" s="129" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="130"/>
-      <c r="K57" s="231">
+      <c r="K57" s="242">
         <f>-C4</f>
         <v>-154314.51999999999</v>
       </c>
-      <c r="L57" s="232"/>
+      <c r="L57" s="243"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="131" t="s">
@@ -9181,29 +9184,29 @@
         <v>19</v>
       </c>
       <c r="F58" s="132">
-        <v>310</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="133">
-        <v>44591</v>
-      </c>
-      <c r="D59" s="208" t="s">
+        <v>44619</v>
+      </c>
+      <c r="D59" s="219" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="209"/>
+      <c r="E59" s="220"/>
       <c r="F59" s="134">
-        <v>154314.51999999999</v>
-      </c>
-      <c r="I59" s="210" t="s">
+        <v>184342.19</v>
+      </c>
+      <c r="I59" s="221" t="s">
         <v>125</v>
       </c>
-      <c r="J59" s="211"/>
-      <c r="K59" s="212">
+      <c r="J59" s="222"/>
+      <c r="K59" s="223">
         <f>K55+K57</f>
-        <v>57733.080000000075</v>
-      </c>
-      <c r="L59" s="212"/>
+        <v>1721491.46</v>
+      </c>
+      <c r="L59" s="223"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="135"/>
@@ -9347,18 +9350,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M40:M41"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -9368,6 +9359,18 @@
     <mergeCell ref="H53:I53"/>
     <mergeCell ref="K53:L53"/>
     <mergeCell ref="M53:N53"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>